<commit_message>
commit 5/23/23 no major changes
</commit_message>
<xml_diff>
--- a/input/references/RATES.xlsx
+++ b/input/references/RATES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba7906c1a1d2a34d/Documents/Work/TTR Project Audit Automation/spreadsheets/references/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/fitzgeralddave_galas_dxc_com/Documents/Documents/Excel/Automations/TMProjectReport/input/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{E5F33A77-2205-4D4C-8182-BDA5175DC061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFE04B21-CDB9-47C9-8D81-DBD635652BDB}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{E5F33A77-2205-4D4C-8182-BDA5175DC061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C2C413-834E-4DED-A125-09D2A24E2449}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1845" windowWidth="23010" windowHeight="12360" xr2:uid="{70D80703-811D-4F1E-A0D0-1D349A2ECF77}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{70D80703-811D-4F1E-A0D0-1D349A2ECF77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -321,9 +321,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64F4B04F-0F97-4FF2-AF49-FE0F2CC7EA05}" name="Table1" displayName="Table1" ref="A1:E212" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:E212" xr:uid="{64F4B04F-0F97-4FF2-AF49-FE0F2CC7EA05}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E212">
-    <sortCondition ref="B1:B212"/>
-  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7A01A2DE-DC89-4633-9C92-3A6349E1C259}" name="Actual Job Level"/>
     <tableColumn id="2" xr3:uid="{3FF15A9C-9E10-4F6E-86A9-6201EF1F1A8C}" name="ActualDXC Job Level"/>
@@ -636,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F3F609-BEB2-442A-A8E4-E3C827BAD00F}">
   <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="O120" sqref="O120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="str">
-        <f>_xlfn.CONCAT(B2,C2)</f>
+        <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(B2,C2)</f>
         <v>L1Argentina</v>
       </c>
       <c r="E2">
@@ -688,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <f>_xlfn.CONCAT(B3,C3)</f>
+        <f t="shared" si="0"/>
         <v>L1Australia</v>
       </c>
       <c r="E3">
@@ -703,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.CONCAT(B4,C4)</f>
+        <f t="shared" si="0"/>
         <v>L1Austria</v>
       </c>
       <c r="E4">
@@ -718,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="str">
-        <f>_xlfn.CONCAT(B5,C5)</f>
+        <f t="shared" si="0"/>
         <v>L1Belgium</v>
       </c>
       <c r="E5">
@@ -733,7 +730,7 @@
         <v>37</v>
       </c>
       <c r="D6" t="str">
-        <f>_xlfn.CONCAT(B6,C6)</f>
+        <f t="shared" si="0"/>
         <v>L1Brazil</v>
       </c>
       <c r="E6">
@@ -748,7 +745,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="str">
-        <f>_xlfn.CONCAT(B7,C7)</f>
+        <f t="shared" si="0"/>
         <v>L1Brazil 2</v>
       </c>
       <c r="E7">
@@ -763,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="str">
-        <f>_xlfn.CONCAT(B8,C8)</f>
+        <f t="shared" si="0"/>
         <v>L1Bulgaria</v>
       </c>
       <c r="E8">
@@ -778,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="str">
-        <f>_xlfn.CONCAT(B9,C9)</f>
+        <f t="shared" si="0"/>
         <v>L1Canada</v>
       </c>
       <c r="E9">
@@ -793,7 +790,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="str">
-        <f>_xlfn.CONCAT(B10,C10)</f>
+        <f t="shared" si="0"/>
         <v>L1China 2</v>
       </c>
       <c r="E10">
@@ -808,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="str">
-        <f>_xlfn.CONCAT(B11,C11)</f>
+        <f t="shared" si="0"/>
         <v>L1Costa Rica</v>
       </c>
       <c r="E11">
@@ -823,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="str">
-        <f>_xlfn.CONCAT(B12,C12)</f>
+        <f t="shared" si="0"/>
         <v>L1France</v>
       </c>
       <c r="E12">
@@ -838,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="str">
-        <f>_xlfn.CONCAT(B13,C13)</f>
+        <f t="shared" si="0"/>
         <v>L1Germany</v>
       </c>
       <c r="E13">
@@ -853,7 +850,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="str">
-        <f>_xlfn.CONCAT(B14,C14)</f>
+        <f t="shared" si="0"/>
         <v>L1Greece</v>
       </c>
       <c r="E14">
@@ -868,7 +865,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="str">
-        <f>_xlfn.CONCAT(B15,C15)</f>
+        <f t="shared" si="0"/>
         <v>L1India</v>
       </c>
       <c r="E15">
@@ -883,7 +880,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="str">
-        <f>_xlfn.CONCAT(B16,C16)</f>
+        <f t="shared" si="0"/>
         <v>L1Ireland</v>
       </c>
       <c r="E16">
@@ -898,7 +895,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="str">
-        <f>_xlfn.CONCAT(B17,C17)</f>
+        <f t="shared" si="0"/>
         <v>L1Israel</v>
       </c>
       <c r="E17">
@@ -913,7 +910,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="str">
-        <f>_xlfn.CONCAT(B18,C18)</f>
+        <f t="shared" si="0"/>
         <v>L1Italy</v>
       </c>
       <c r="E18">
@@ -928,7 +925,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="str">
-        <f>_xlfn.CONCAT(B19,C19)</f>
+        <f t="shared" si="0"/>
         <v>L1Japan</v>
       </c>
       <c r="E19">
@@ -943,7 +940,7 @@
         <v>17</v>
       </c>
       <c r="D20" t="str">
-        <f>_xlfn.CONCAT(B20,C20)</f>
+        <f t="shared" si="0"/>
         <v>L1Malaysia</v>
       </c>
       <c r="E20">
@@ -958,7 +955,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="str">
-        <f>_xlfn.CONCAT(B21,C21)</f>
+        <f t="shared" si="0"/>
         <v>L1Mexico</v>
       </c>
       <c r="E21">
@@ -973,7 +970,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="str">
-        <f>_xlfn.CONCAT(B22,C22)</f>
+        <f t="shared" si="0"/>
         <v>L1Netherlands</v>
       </c>
       <c r="E22">
@@ -988,7 +985,7 @@
         <v>38</v>
       </c>
       <c r="D23" t="str">
-        <f>_xlfn.CONCAT(B23,C23)</f>
+        <f t="shared" si="0"/>
         <v>L1P.R.C.</v>
       </c>
       <c r="E23">
@@ -1003,7 +1000,7 @@
         <v>20</v>
       </c>
       <c r="D24" t="str">
-        <f>_xlfn.CONCAT(B24,C24)</f>
+        <f t="shared" si="0"/>
         <v>L1Philippines</v>
       </c>
       <c r="E24">
@@ -1018,7 +1015,7 @@
         <v>40</v>
       </c>
       <c r="D25" t="str">
-        <f>_xlfn.CONCAT(B25,C25)</f>
+        <f t="shared" si="0"/>
         <v>L1Philippines 1</v>
       </c>
       <c r="E25">
@@ -1033,7 +1030,7 @@
         <v>21</v>
       </c>
       <c r="D26" t="str">
-        <f>_xlfn.CONCAT(B26,C26)</f>
+        <f t="shared" si="0"/>
         <v>L1Poland</v>
       </c>
       <c r="E26">
@@ -1048,7 +1045,7 @@
         <v>22</v>
       </c>
       <c r="D27" t="str">
-        <f>_xlfn.CONCAT(B27,C27)</f>
+        <f t="shared" si="0"/>
         <v>L1Puerto Rico</v>
       </c>
       <c r="E27">
@@ -1063,7 +1060,7 @@
         <v>23</v>
       </c>
       <c r="D28" t="str">
-        <f>_xlfn.CONCAT(B28,C28)</f>
+        <f t="shared" si="0"/>
         <v>L1Romania</v>
       </c>
       <c r="E28">
@@ -1078,7 +1075,7 @@
         <v>24</v>
       </c>
       <c r="D29" t="str">
-        <f>_xlfn.CONCAT(B29,C29)</f>
+        <f t="shared" si="0"/>
         <v>L1Saudi Arabia</v>
       </c>
       <c r="E29">
@@ -1093,7 +1090,7 @@
         <v>25</v>
       </c>
       <c r="D30" t="str">
-        <f>_xlfn.CONCAT(B30,C30)</f>
+        <f t="shared" si="0"/>
         <v>L1Serbia</v>
       </c>
       <c r="E30">
@@ -1108,7 +1105,7 @@
         <v>26</v>
       </c>
       <c r="D31" t="str">
-        <f>_xlfn.CONCAT(B31,C31)</f>
+        <f t="shared" si="0"/>
         <v>L1Singapore</v>
       </c>
       <c r="E31">
@@ -1123,7 +1120,7 @@
         <v>27</v>
       </c>
       <c r="D32" t="str">
-        <f>_xlfn.CONCAT(B32,C32)</f>
+        <f t="shared" si="0"/>
         <v>L1Slovakia</v>
       </c>
       <c r="E32">
@@ -1138,7 +1135,7 @@
         <v>28</v>
       </c>
       <c r="D33" t="str">
-        <f>_xlfn.CONCAT(B33,C33)</f>
+        <f t="shared" si="0"/>
         <v>L1Spain</v>
       </c>
       <c r="E33">
@@ -1153,7 +1150,7 @@
         <v>39</v>
       </c>
       <c r="D34" t="str">
-        <f>_xlfn.CONCAT(B34,C34)</f>
+        <f t="shared" si="0"/>
         <v>L1United Arab Emirates</v>
       </c>
       <c r="E34">
@@ -1168,7 +1165,7 @@
         <v>29</v>
       </c>
       <c r="D35" t="str">
-        <f>_xlfn.CONCAT(B35,C35)</f>
+        <f t="shared" si="0"/>
         <v>L1United Kingdom</v>
       </c>
       <c r="E35">
@@ -1183,7 +1180,7 @@
         <v>30</v>
       </c>
       <c r="D36" t="str">
-        <f>_xlfn.CONCAT(B36,C36)</f>
+        <f t="shared" si="0"/>
         <v>L1United States</v>
       </c>
       <c r="E36">
@@ -1201,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="str">
-        <f>_xlfn.CONCAT(B37,C37)</f>
+        <f t="shared" si="0"/>
         <v>L3Argentina</v>
       </c>
       <c r="E37">
@@ -1219,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="str">
-        <f>_xlfn.CONCAT(B38,C38)</f>
+        <f t="shared" si="0"/>
         <v>L3Australia</v>
       </c>
       <c r="E38">
@@ -1237,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="str">
-        <f>_xlfn.CONCAT(B39,C39)</f>
+        <f t="shared" si="0"/>
         <v>L3Austria</v>
       </c>
       <c r="E39">
@@ -1255,7 +1252,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="str">
-        <f>_xlfn.CONCAT(B40,C40)</f>
+        <f t="shared" si="0"/>
         <v>L3Belgium</v>
       </c>
       <c r="E40">
@@ -1273,7 +1270,7 @@
         <v>37</v>
       </c>
       <c r="D41" t="str">
-        <f>_xlfn.CONCAT(B41,C41)</f>
+        <f t="shared" si="0"/>
         <v>L3Brazil</v>
       </c>
       <c r="E41">
@@ -1291,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="D42" t="str">
-        <f>_xlfn.CONCAT(B42,C42)</f>
+        <f t="shared" si="0"/>
         <v>L3Brazil 2</v>
       </c>
       <c r="E42">
@@ -1309,7 +1306,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="str">
-        <f>_xlfn.CONCAT(B43,C43)</f>
+        <f t="shared" si="0"/>
         <v>L3Bulgaria</v>
       </c>
       <c r="E43">
@@ -1327,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="D44" t="str">
-        <f>_xlfn.CONCAT(B44,C44)</f>
+        <f t="shared" si="0"/>
         <v>L3Canada</v>
       </c>
       <c r="E44">
@@ -1345,7 +1342,7 @@
         <v>7</v>
       </c>
       <c r="D45" t="str">
-        <f>_xlfn.CONCAT(B45,C45)</f>
+        <f t="shared" si="0"/>
         <v>L3China 2</v>
       </c>
       <c r="E45">
@@ -1363,7 +1360,7 @@
         <v>8</v>
       </c>
       <c r="D46" t="str">
-        <f>_xlfn.CONCAT(B46,C46)</f>
+        <f t="shared" si="0"/>
         <v>L3Costa Rica</v>
       </c>
       <c r="E46">
@@ -1381,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="D47" t="str">
-        <f>_xlfn.CONCAT(B47,C47)</f>
+        <f t="shared" si="0"/>
         <v>L3France</v>
       </c>
       <c r="E47">
@@ -1399,7 +1396,7 @@
         <v>10</v>
       </c>
       <c r="D48" t="str">
-        <f>_xlfn.CONCAT(B48,C48)</f>
+        <f t="shared" si="0"/>
         <v>L3Germany</v>
       </c>
       <c r="E48">
@@ -1417,7 +1414,7 @@
         <v>11</v>
       </c>
       <c r="D49" t="str">
-        <f>_xlfn.CONCAT(B49,C49)</f>
+        <f t="shared" si="0"/>
         <v>L3Greece</v>
       </c>
       <c r="E49">
@@ -1435,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="D50" t="str">
-        <f>_xlfn.CONCAT(B50,C50)</f>
+        <f t="shared" si="0"/>
         <v>L3India</v>
       </c>
       <c r="E50">
@@ -1453,7 +1450,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="str">
-        <f>_xlfn.CONCAT(B51,C51)</f>
+        <f t="shared" si="0"/>
         <v>L3Ireland</v>
       </c>
       <c r="E51">
@@ -1471,7 +1468,7 @@
         <v>14</v>
       </c>
       <c r="D52" t="str">
-        <f>_xlfn.CONCAT(B52,C52)</f>
+        <f t="shared" si="0"/>
         <v>L3Israel</v>
       </c>
       <c r="E52">
@@ -1489,7 +1486,7 @@
         <v>15</v>
       </c>
       <c r="D53" t="str">
-        <f>_xlfn.CONCAT(B53,C53)</f>
+        <f t="shared" si="0"/>
         <v>L3Italy</v>
       </c>
       <c r="E53">
@@ -1507,7 +1504,7 @@
         <v>16</v>
       </c>
       <c r="D54" t="str">
-        <f>_xlfn.CONCAT(B54,C54)</f>
+        <f t="shared" si="0"/>
         <v>L3Japan</v>
       </c>
       <c r="E54">
@@ -1525,7 +1522,7 @@
         <v>17</v>
       </c>
       <c r="D55" t="str">
-        <f>_xlfn.CONCAT(B55,C55)</f>
+        <f t="shared" si="0"/>
         <v>L3Malaysia</v>
       </c>
       <c r="E55">
@@ -1543,7 +1540,7 @@
         <v>18</v>
       </c>
       <c r="D56" t="str">
-        <f>_xlfn.CONCAT(B56,C56)</f>
+        <f t="shared" si="0"/>
         <v>L3Mexico</v>
       </c>
       <c r="E56">
@@ -1561,7 +1558,7 @@
         <v>19</v>
       </c>
       <c r="D57" t="str">
-        <f>_xlfn.CONCAT(B57,C57)</f>
+        <f t="shared" si="0"/>
         <v>L3Netherlands</v>
       </c>
       <c r="E57">
@@ -1579,7 +1576,7 @@
         <v>38</v>
       </c>
       <c r="D58" t="str">
-        <f>_xlfn.CONCAT(B58,C58)</f>
+        <f t="shared" si="0"/>
         <v>L3P.R.C.</v>
       </c>
       <c r="E58">
@@ -1597,7 +1594,7 @@
         <v>20</v>
       </c>
       <c r="D59" t="str">
-        <f>_xlfn.CONCAT(B59,C59)</f>
+        <f t="shared" si="0"/>
         <v>L3Philippines</v>
       </c>
       <c r="E59">
@@ -1615,7 +1612,7 @@
         <v>40</v>
       </c>
       <c r="D60" t="str">
-        <f>_xlfn.CONCAT(B60,C60)</f>
+        <f t="shared" si="0"/>
         <v>L3Philippines 1</v>
       </c>
       <c r="E60">
@@ -1633,7 +1630,7 @@
         <v>21</v>
       </c>
       <c r="D61" t="str">
-        <f>_xlfn.CONCAT(B61,C61)</f>
+        <f t="shared" si="0"/>
         <v>L3Poland</v>
       </c>
       <c r="E61">
@@ -1651,7 +1648,7 @@
         <v>22</v>
       </c>
       <c r="D62" t="str">
-        <f>_xlfn.CONCAT(B62,C62)</f>
+        <f t="shared" si="0"/>
         <v>L3Puerto Rico</v>
       </c>
       <c r="E62">
@@ -1669,7 +1666,7 @@
         <v>23</v>
       </c>
       <c r="D63" t="str">
-        <f>_xlfn.CONCAT(B63,C63)</f>
+        <f t="shared" si="0"/>
         <v>L3Romania</v>
       </c>
       <c r="E63">
@@ -1687,7 +1684,7 @@
         <v>24</v>
       </c>
       <c r="D64" t="str">
-        <f>_xlfn.CONCAT(B64,C64)</f>
+        <f t="shared" si="0"/>
         <v>L3Saudi Arabia</v>
       </c>
       <c r="E64">
@@ -1705,7 +1702,7 @@
         <v>25</v>
       </c>
       <c r="D65" t="str">
-        <f>_xlfn.CONCAT(B65,C65)</f>
+        <f t="shared" si="0"/>
         <v>L3Serbia</v>
       </c>
       <c r="E65">
@@ -1723,7 +1720,7 @@
         <v>26</v>
       </c>
       <c r="D66" t="str">
-        <f>_xlfn.CONCAT(B66,C66)</f>
+        <f t="shared" ref="D66:D129" si="1">_xlfn.CONCAT(B66,C66)</f>
         <v>L3Singapore</v>
       </c>
       <c r="E66">
@@ -1741,7 +1738,7 @@
         <v>27</v>
       </c>
       <c r="D67" t="str">
-        <f>_xlfn.CONCAT(B67,C67)</f>
+        <f t="shared" si="1"/>
         <v>L3Slovakia</v>
       </c>
       <c r="E67">
@@ -1759,7 +1756,7 @@
         <v>28</v>
       </c>
       <c r="D68" t="str">
-        <f>_xlfn.CONCAT(B68,C68)</f>
+        <f t="shared" si="1"/>
         <v>L3Spain</v>
       </c>
       <c r="E68">
@@ -1777,7 +1774,7 @@
         <v>39</v>
       </c>
       <c r="D69" t="str">
-        <f>_xlfn.CONCAT(B69,C69)</f>
+        <f t="shared" si="1"/>
         <v>L3United Arab Emirates</v>
       </c>
       <c r="E69">
@@ -1795,7 +1792,7 @@
         <v>29</v>
       </c>
       <c r="D70" t="str">
-        <f>_xlfn.CONCAT(B70,C70)</f>
+        <f t="shared" si="1"/>
         <v>L3United Kingdom</v>
       </c>
       <c r="E70">
@@ -1813,7 +1810,7 @@
         <v>30</v>
       </c>
       <c r="D71" t="str">
-        <f>_xlfn.CONCAT(B71,C71)</f>
+        <f t="shared" si="1"/>
         <v>L3United States</v>
       </c>
       <c r="E71">
@@ -1831,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="D72" t="str">
-        <f>_xlfn.CONCAT(B72,C72)</f>
+        <f t="shared" si="1"/>
         <v>L4Argentina</v>
       </c>
       <c r="E72">
@@ -1849,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="D73" t="str">
-        <f>_xlfn.CONCAT(B73,C73)</f>
+        <f t="shared" si="1"/>
         <v>L4Australia</v>
       </c>
       <c r="E73">
@@ -1867,7 +1864,7 @@
         <v>2</v>
       </c>
       <c r="D74" t="str">
-        <f>_xlfn.CONCAT(B74,C74)</f>
+        <f t="shared" si="1"/>
         <v>L4Austria</v>
       </c>
       <c r="E74">
@@ -1885,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="D75" t="str">
-        <f>_xlfn.CONCAT(B75,C75)</f>
+        <f t="shared" si="1"/>
         <v>L4Belgium</v>
       </c>
       <c r="E75">
@@ -1903,7 +1900,7 @@
         <v>37</v>
       </c>
       <c r="D76" t="str">
-        <f>_xlfn.CONCAT(B76,C76)</f>
+        <f t="shared" si="1"/>
         <v>L4Brazil</v>
       </c>
       <c r="E76">
@@ -1921,7 +1918,7 @@
         <v>4</v>
       </c>
       <c r="D77" t="str">
-        <f>_xlfn.CONCAT(B77,C77)</f>
+        <f t="shared" si="1"/>
         <v>L4Brazil 2</v>
       </c>
       <c r="E77">
@@ -1939,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="D78" t="str">
-        <f>_xlfn.CONCAT(B78,C78)</f>
+        <f t="shared" si="1"/>
         <v>L4Bulgaria</v>
       </c>
       <c r="E78">
@@ -1957,7 +1954,7 @@
         <v>6</v>
       </c>
       <c r="D79" t="str">
-        <f>_xlfn.CONCAT(B79,C79)</f>
+        <f t="shared" si="1"/>
         <v>L4Canada</v>
       </c>
       <c r="E79">
@@ -1975,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="D80" t="str">
-        <f>_xlfn.CONCAT(B80,C80)</f>
+        <f t="shared" si="1"/>
         <v>L4China 2</v>
       </c>
       <c r="E80">
@@ -1993,7 +1990,7 @@
         <v>8</v>
       </c>
       <c r="D81" t="str">
-        <f>_xlfn.CONCAT(B81,C81)</f>
+        <f t="shared" si="1"/>
         <v>L4Costa Rica</v>
       </c>
       <c r="E81">
@@ -2011,7 +2008,7 @@
         <v>9</v>
       </c>
       <c r="D82" t="str">
-        <f>_xlfn.CONCAT(B82,C82)</f>
+        <f t="shared" si="1"/>
         <v>L4France</v>
       </c>
       <c r="E82">
@@ -2029,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="D83" t="str">
-        <f>_xlfn.CONCAT(B83,C83)</f>
+        <f t="shared" si="1"/>
         <v>L4Germany</v>
       </c>
       <c r="E83">
@@ -2047,7 +2044,7 @@
         <v>11</v>
       </c>
       <c r="D84" t="str">
-        <f>_xlfn.CONCAT(B84,C84)</f>
+        <f t="shared" si="1"/>
         <v>L4Greece</v>
       </c>
       <c r="E84">
@@ -2065,7 +2062,7 @@
         <v>12</v>
       </c>
       <c r="D85" t="str">
-        <f>_xlfn.CONCAT(B85,C85)</f>
+        <f t="shared" si="1"/>
         <v>L4India</v>
       </c>
       <c r="E85">
@@ -2083,7 +2080,7 @@
         <v>12</v>
       </c>
       <c r="D86" t="str">
-        <f>_xlfn.CONCAT(B86,C86)</f>
+        <f t="shared" si="1"/>
         <v>L4India</v>
       </c>
       <c r="E86">
@@ -2101,7 +2098,7 @@
         <v>13</v>
       </c>
       <c r="D87" t="str">
-        <f>_xlfn.CONCAT(B87,C87)</f>
+        <f t="shared" si="1"/>
         <v>L4Ireland</v>
       </c>
       <c r="E87">
@@ -2119,7 +2116,7 @@
         <v>14</v>
       </c>
       <c r="D88" t="str">
-        <f>_xlfn.CONCAT(B88,C88)</f>
+        <f t="shared" si="1"/>
         <v>L4Israel</v>
       </c>
       <c r="E88">
@@ -2137,7 +2134,7 @@
         <v>15</v>
       </c>
       <c r="D89" t="str">
-        <f>_xlfn.CONCAT(B89,C89)</f>
+        <f t="shared" si="1"/>
         <v>L4Italy</v>
       </c>
       <c r="E89">
@@ -2155,7 +2152,7 @@
         <v>16</v>
       </c>
       <c r="D90" t="str">
-        <f>_xlfn.CONCAT(B90,C90)</f>
+        <f t="shared" si="1"/>
         <v>L4Japan</v>
       </c>
       <c r="E90">
@@ -2173,7 +2170,7 @@
         <v>17</v>
       </c>
       <c r="D91" t="str">
-        <f>_xlfn.CONCAT(B91,C91)</f>
+        <f t="shared" si="1"/>
         <v>L4Malaysia</v>
       </c>
       <c r="E91">
@@ -2191,7 +2188,7 @@
         <v>18</v>
       </c>
       <c r="D92" t="str">
-        <f>_xlfn.CONCAT(B92,C92)</f>
+        <f t="shared" si="1"/>
         <v>L4Mexico</v>
       </c>
       <c r="E92">
@@ -2209,7 +2206,7 @@
         <v>19</v>
       </c>
       <c r="D93" t="str">
-        <f>_xlfn.CONCAT(B93,C93)</f>
+        <f t="shared" si="1"/>
         <v>L4Netherlands</v>
       </c>
       <c r="E93">
@@ -2227,7 +2224,7 @@
         <v>38</v>
       </c>
       <c r="D94" t="str">
-        <f>_xlfn.CONCAT(B94,C94)</f>
+        <f t="shared" si="1"/>
         <v>L4P.R.C.</v>
       </c>
       <c r="E94">
@@ -2245,7 +2242,7 @@
         <v>20</v>
       </c>
       <c r="D95" t="str">
-        <f>_xlfn.CONCAT(B95,C95)</f>
+        <f t="shared" si="1"/>
         <v>L4Philippines</v>
       </c>
       <c r="E95">
@@ -2263,7 +2260,7 @@
         <v>40</v>
       </c>
       <c r="D96" t="str">
-        <f>_xlfn.CONCAT(B96,C96)</f>
+        <f t="shared" si="1"/>
         <v>L4Philippines 1</v>
       </c>
       <c r="E96">
@@ -2281,7 +2278,7 @@
         <v>21</v>
       </c>
       <c r="D97" t="str">
-        <f>_xlfn.CONCAT(B97,C97)</f>
+        <f t="shared" si="1"/>
         <v>L4Poland</v>
       </c>
       <c r="E97">
@@ -2299,7 +2296,7 @@
         <v>22</v>
       </c>
       <c r="D98" t="str">
-        <f>_xlfn.CONCAT(B98,C98)</f>
+        <f t="shared" si="1"/>
         <v>L4Puerto Rico</v>
       </c>
       <c r="E98">
@@ -2317,7 +2314,7 @@
         <v>23</v>
       </c>
       <c r="D99" t="str">
-        <f>_xlfn.CONCAT(B99,C99)</f>
+        <f t="shared" si="1"/>
         <v>L4Romania</v>
       </c>
       <c r="E99">
@@ -2335,7 +2332,7 @@
         <v>24</v>
       </c>
       <c r="D100" t="str">
-        <f>_xlfn.CONCAT(B100,C100)</f>
+        <f t="shared" si="1"/>
         <v>L4Saudi Arabia</v>
       </c>
       <c r="E100">
@@ -2353,7 +2350,7 @@
         <v>25</v>
       </c>
       <c r="D101" t="str">
-        <f>_xlfn.CONCAT(B101,C101)</f>
+        <f t="shared" si="1"/>
         <v>L4Serbia</v>
       </c>
       <c r="E101">
@@ -2371,7 +2368,7 @@
         <v>26</v>
       </c>
       <c r="D102" t="str">
-        <f>_xlfn.CONCAT(B102,C102)</f>
+        <f t="shared" si="1"/>
         <v>L4Singapore</v>
       </c>
       <c r="E102">
@@ -2389,7 +2386,7 @@
         <v>27</v>
       </c>
       <c r="D103" t="str">
-        <f>_xlfn.CONCAT(B103,C103)</f>
+        <f t="shared" si="1"/>
         <v>L4Slovakia</v>
       </c>
       <c r="E103">
@@ -2407,7 +2404,7 @@
         <v>28</v>
       </c>
       <c r="D104" t="str">
-        <f>_xlfn.CONCAT(B104,C104)</f>
+        <f t="shared" si="1"/>
         <v>L4Spain</v>
       </c>
       <c r="E104">
@@ -2425,7 +2422,7 @@
         <v>39</v>
       </c>
       <c r="D105" t="str">
-        <f>_xlfn.CONCAT(B105,C105)</f>
+        <f t="shared" si="1"/>
         <v>L4United Arab Emirates</v>
       </c>
       <c r="E105">
@@ -2443,7 +2440,7 @@
         <v>29</v>
       </c>
       <c r="D106" t="str">
-        <f>_xlfn.CONCAT(B106,C106)</f>
+        <f t="shared" si="1"/>
         <v>L4United Kingdom</v>
       </c>
       <c r="E106">
@@ -2461,7 +2458,7 @@
         <v>30</v>
       </c>
       <c r="D107" t="str">
-        <f>_xlfn.CONCAT(B107,C107)</f>
+        <f t="shared" si="1"/>
         <v>L4United States</v>
       </c>
       <c r="E107">
@@ -2479,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="D108" t="str">
-        <f>_xlfn.CONCAT(B108,C108)</f>
+        <f t="shared" si="1"/>
         <v>L5Argentina</v>
       </c>
       <c r="E108">
@@ -2497,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="D109" t="str">
-        <f>_xlfn.CONCAT(B109,C109)</f>
+        <f t="shared" si="1"/>
         <v>L5Australia</v>
       </c>
       <c r="E109">
@@ -2515,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="D110" t="str">
-        <f>_xlfn.CONCAT(B110,C110)</f>
+        <f t="shared" si="1"/>
         <v>L5Austria</v>
       </c>
       <c r="E110">
@@ -2533,7 +2530,7 @@
         <v>3</v>
       </c>
       <c r="D111" t="str">
-        <f>_xlfn.CONCAT(B111,C111)</f>
+        <f t="shared" si="1"/>
         <v>L5Belgium</v>
       </c>
       <c r="E111">
@@ -2551,7 +2548,7 @@
         <v>37</v>
       </c>
       <c r="D112" t="str">
-        <f>_xlfn.CONCAT(B112,C112)</f>
+        <f t="shared" si="1"/>
         <v>L5Brazil</v>
       </c>
       <c r="E112">
@@ -2569,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="D113" t="str">
-        <f>_xlfn.CONCAT(B113,C113)</f>
+        <f t="shared" si="1"/>
         <v>L5Brazil 2</v>
       </c>
       <c r="E113">
@@ -2587,7 +2584,7 @@
         <v>5</v>
       </c>
       <c r="D114" t="str">
-        <f>_xlfn.CONCAT(B114,C114)</f>
+        <f t="shared" si="1"/>
         <v>L5Bulgaria</v>
       </c>
       <c r="E114">
@@ -2605,7 +2602,7 @@
         <v>6</v>
       </c>
       <c r="D115" t="str">
-        <f>_xlfn.CONCAT(B115,C115)</f>
+        <f t="shared" si="1"/>
         <v>L5Canada</v>
       </c>
       <c r="E115">
@@ -2623,7 +2620,7 @@
         <v>7</v>
       </c>
       <c r="D116" t="str">
-        <f>_xlfn.CONCAT(B116,C116)</f>
+        <f t="shared" si="1"/>
         <v>L5China 2</v>
       </c>
       <c r="E116">
@@ -2641,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="D117" t="str">
-        <f>_xlfn.CONCAT(B117,C117)</f>
+        <f t="shared" si="1"/>
         <v>L5Costa Rica</v>
       </c>
       <c r="E117">
@@ -2659,7 +2656,7 @@
         <v>9</v>
       </c>
       <c r="D118" t="str">
-        <f>_xlfn.CONCAT(B118,C118)</f>
+        <f t="shared" si="1"/>
         <v>L5France</v>
       </c>
       <c r="E118">
@@ -2677,7 +2674,7 @@
         <v>10</v>
       </c>
       <c r="D119" t="str">
-        <f>_xlfn.CONCAT(B119,C119)</f>
+        <f t="shared" si="1"/>
         <v>L5Germany</v>
       </c>
       <c r="E119">
@@ -2695,7 +2692,7 @@
         <v>11</v>
       </c>
       <c r="D120" t="str">
-        <f>_xlfn.CONCAT(B120,C120)</f>
+        <f t="shared" si="1"/>
         <v>L5Greece</v>
       </c>
       <c r="E120">
@@ -2713,7 +2710,7 @@
         <v>12</v>
       </c>
       <c r="D121" t="str">
-        <f>_xlfn.CONCAT(B121,C121)</f>
+        <f t="shared" si="1"/>
         <v>L5India</v>
       </c>
       <c r="E121">
@@ -2731,7 +2728,7 @@
         <v>13</v>
       </c>
       <c r="D122" t="str">
-        <f>_xlfn.CONCAT(B122,C122)</f>
+        <f t="shared" si="1"/>
         <v>L5Ireland</v>
       </c>
       <c r="E122">
@@ -2749,7 +2746,7 @@
         <v>14</v>
       </c>
       <c r="D123" t="str">
-        <f>_xlfn.CONCAT(B123,C123)</f>
+        <f t="shared" si="1"/>
         <v>L5Israel</v>
       </c>
       <c r="E123">
@@ -2767,7 +2764,7 @@
         <v>15</v>
       </c>
       <c r="D124" t="str">
-        <f>_xlfn.CONCAT(B124,C124)</f>
+        <f t="shared" si="1"/>
         <v>L5Italy</v>
       </c>
       <c r="E124">
@@ -2785,7 +2782,7 @@
         <v>16</v>
       </c>
       <c r="D125" t="str">
-        <f>_xlfn.CONCAT(B125,C125)</f>
+        <f t="shared" si="1"/>
         <v>L5Japan</v>
       </c>
       <c r="E125">
@@ -2803,7 +2800,7 @@
         <v>17</v>
       </c>
       <c r="D126" t="str">
-        <f>_xlfn.CONCAT(B126,C126)</f>
+        <f t="shared" si="1"/>
         <v>L5Malaysia</v>
       </c>
       <c r="E126">
@@ -2821,7 +2818,7 @@
         <v>18</v>
       </c>
       <c r="D127" t="str">
-        <f>_xlfn.CONCAT(B127,C127)</f>
+        <f t="shared" si="1"/>
         <v>L5Mexico</v>
       </c>
       <c r="E127">
@@ -2839,7 +2836,7 @@
         <v>19</v>
       </c>
       <c r="D128" t="str">
-        <f>_xlfn.CONCAT(B128,C128)</f>
+        <f t="shared" si="1"/>
         <v>L5Netherlands</v>
       </c>
       <c r="E128">
@@ -2857,7 +2854,7 @@
         <v>38</v>
       </c>
       <c r="D129" t="str">
-        <f>_xlfn.CONCAT(B129,C129)</f>
+        <f t="shared" si="1"/>
         <v>L5P.R.C.</v>
       </c>
       <c r="E129">
@@ -2875,7 +2872,7 @@
         <v>20</v>
       </c>
       <c r="D130" t="str">
-        <f>_xlfn.CONCAT(B130,C130)</f>
+        <f t="shared" ref="D130:D193" si="2">_xlfn.CONCAT(B130,C130)</f>
         <v>L5Philippines</v>
       </c>
       <c r="E130">
@@ -2893,7 +2890,7 @@
         <v>40</v>
       </c>
       <c r="D131" t="str">
-        <f>_xlfn.CONCAT(B131,C131)</f>
+        <f t="shared" si="2"/>
         <v>L5Philippines 1</v>
       </c>
       <c r="E131">
@@ -2911,7 +2908,7 @@
         <v>21</v>
       </c>
       <c r="D132" t="str">
-        <f>_xlfn.CONCAT(B132,C132)</f>
+        <f t="shared" si="2"/>
         <v>L5Poland</v>
       </c>
       <c r="E132">
@@ -2929,7 +2926,7 @@
         <v>22</v>
       </c>
       <c r="D133" t="str">
-        <f>_xlfn.CONCAT(B133,C133)</f>
+        <f t="shared" si="2"/>
         <v>L5Puerto Rico</v>
       </c>
       <c r="E133">
@@ -2947,7 +2944,7 @@
         <v>23</v>
       </c>
       <c r="D134" t="str">
-        <f>_xlfn.CONCAT(B134,C134)</f>
+        <f t="shared" si="2"/>
         <v>L5Romania</v>
       </c>
       <c r="E134">
@@ -2965,7 +2962,7 @@
         <v>24</v>
       </c>
       <c r="D135" t="str">
-        <f>_xlfn.CONCAT(B135,C135)</f>
+        <f t="shared" si="2"/>
         <v>L5Saudi Arabia</v>
       </c>
       <c r="E135">
@@ -2983,7 +2980,7 @@
         <v>25</v>
       </c>
       <c r="D136" t="str">
-        <f>_xlfn.CONCAT(B136,C136)</f>
+        <f t="shared" si="2"/>
         <v>L5Serbia</v>
       </c>
       <c r="E136">
@@ -3001,7 +2998,7 @@
         <v>26</v>
       </c>
       <c r="D137" t="str">
-        <f>_xlfn.CONCAT(B137,C137)</f>
+        <f t="shared" si="2"/>
         <v>L5Singapore</v>
       </c>
       <c r="E137">
@@ -3019,7 +3016,7 @@
         <v>27</v>
       </c>
       <c r="D138" t="str">
-        <f>_xlfn.CONCAT(B138,C138)</f>
+        <f t="shared" si="2"/>
         <v>L5Slovakia</v>
       </c>
       <c r="E138">
@@ -3037,7 +3034,7 @@
         <v>28</v>
       </c>
       <c r="D139" t="str">
-        <f>_xlfn.CONCAT(B139,C139)</f>
+        <f t="shared" si="2"/>
         <v>L5Spain</v>
       </c>
       <c r="E139">
@@ -3055,7 +3052,7 @@
         <v>39</v>
       </c>
       <c r="D140" t="str">
-        <f>_xlfn.CONCAT(B140,C140)</f>
+        <f t="shared" si="2"/>
         <v>L5United Arab Emirates</v>
       </c>
       <c r="E140">
@@ -3073,7 +3070,7 @@
         <v>29</v>
       </c>
       <c r="D141" t="str">
-        <f>_xlfn.CONCAT(B141,C141)</f>
+        <f t="shared" si="2"/>
         <v>L5United Kingdom</v>
       </c>
       <c r="E141">
@@ -3091,7 +3088,7 @@
         <v>30</v>
       </c>
       <c r="D142" t="str">
-        <f>_xlfn.CONCAT(B142,C142)</f>
+        <f t="shared" si="2"/>
         <v>L5United States</v>
       </c>
       <c r="E142">
@@ -3109,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="D143" t="str">
-        <f>_xlfn.CONCAT(B143,C143)</f>
+        <f t="shared" si="2"/>
         <v>L6Argentina</v>
       </c>
       <c r="E143">
@@ -3127,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="D144" t="str">
-        <f>_xlfn.CONCAT(B144,C144)</f>
+        <f t="shared" si="2"/>
         <v>L6Australia</v>
       </c>
       <c r="E144">
@@ -3145,7 +3142,7 @@
         <v>2</v>
       </c>
       <c r="D145" t="str">
-        <f>_xlfn.CONCAT(B145,C145)</f>
+        <f t="shared" si="2"/>
         <v>L6Austria</v>
       </c>
       <c r="E145">
@@ -3163,7 +3160,7 @@
         <v>3</v>
       </c>
       <c r="D146" t="str">
-        <f>_xlfn.CONCAT(B146,C146)</f>
+        <f t="shared" si="2"/>
         <v>L6Belgium</v>
       </c>
       <c r="E146">
@@ -3181,7 +3178,7 @@
         <v>37</v>
       </c>
       <c r="D147" t="str">
-        <f>_xlfn.CONCAT(B147,C147)</f>
+        <f t="shared" si="2"/>
         <v>L6Brazil</v>
       </c>
       <c r="E147">
@@ -3199,7 +3196,7 @@
         <v>4</v>
       </c>
       <c r="D148" t="str">
-        <f>_xlfn.CONCAT(B148,C148)</f>
+        <f t="shared" si="2"/>
         <v>L6Brazil 2</v>
       </c>
       <c r="E148">
@@ -3217,7 +3214,7 @@
         <v>5</v>
       </c>
       <c r="D149" t="str">
-        <f>_xlfn.CONCAT(B149,C149)</f>
+        <f t="shared" si="2"/>
         <v>L6Bulgaria</v>
       </c>
       <c r="E149">
@@ -3235,7 +3232,7 @@
         <v>6</v>
       </c>
       <c r="D150" t="str">
-        <f>_xlfn.CONCAT(B150,C150)</f>
+        <f t="shared" si="2"/>
         <v>L6Canada</v>
       </c>
       <c r="E150">
@@ -3253,7 +3250,7 @@
         <v>7</v>
       </c>
       <c r="D151" t="str">
-        <f>_xlfn.CONCAT(B151,C151)</f>
+        <f t="shared" si="2"/>
         <v>L6China 2</v>
       </c>
       <c r="E151">
@@ -3271,7 +3268,7 @@
         <v>8</v>
       </c>
       <c r="D152" t="str">
-        <f>_xlfn.CONCAT(B152,C152)</f>
+        <f t="shared" si="2"/>
         <v>L6Costa Rica</v>
       </c>
       <c r="E152">
@@ -3289,7 +3286,7 @@
         <v>9</v>
       </c>
       <c r="D153" t="str">
-        <f>_xlfn.CONCAT(B153,C153)</f>
+        <f t="shared" si="2"/>
         <v>L6France</v>
       </c>
       <c r="E153">
@@ -3307,7 +3304,7 @@
         <v>10</v>
       </c>
       <c r="D154" t="str">
-        <f>_xlfn.CONCAT(B154,C154)</f>
+        <f t="shared" si="2"/>
         <v>L6Germany</v>
       </c>
       <c r="E154">
@@ -3325,7 +3322,7 @@
         <v>11</v>
       </c>
       <c r="D155" t="str">
-        <f>_xlfn.CONCAT(B155,C155)</f>
+        <f t="shared" si="2"/>
         <v>L6Greece</v>
       </c>
       <c r="E155">
@@ -3343,7 +3340,7 @@
         <v>12</v>
       </c>
       <c r="D156" t="str">
-        <f>_xlfn.CONCAT(B156,C156)</f>
+        <f t="shared" si="2"/>
         <v>L6India</v>
       </c>
       <c r="E156">
@@ -3361,7 +3358,7 @@
         <v>13</v>
       </c>
       <c r="D157" t="str">
-        <f>_xlfn.CONCAT(B157,C157)</f>
+        <f t="shared" si="2"/>
         <v>L6Ireland</v>
       </c>
       <c r="E157">
@@ -3379,7 +3376,7 @@
         <v>14</v>
       </c>
       <c r="D158" t="str">
-        <f>_xlfn.CONCAT(B158,C158)</f>
+        <f t="shared" si="2"/>
         <v>L6Israel</v>
       </c>
       <c r="E158">
@@ -3397,7 +3394,7 @@
         <v>15</v>
       </c>
       <c r="D159" t="str">
-        <f>_xlfn.CONCAT(B159,C159)</f>
+        <f t="shared" si="2"/>
         <v>L6Italy</v>
       </c>
       <c r="E159">
@@ -3415,7 +3412,7 @@
         <v>16</v>
       </c>
       <c r="D160" t="str">
-        <f>_xlfn.CONCAT(B160,C160)</f>
+        <f t="shared" si="2"/>
         <v>L6Japan</v>
       </c>
       <c r="E160">
@@ -3433,7 +3430,7 @@
         <v>17</v>
       </c>
       <c r="D161" t="str">
-        <f>_xlfn.CONCAT(B161,C161)</f>
+        <f t="shared" si="2"/>
         <v>L6Malaysia</v>
       </c>
       <c r="E161">
@@ -3451,7 +3448,7 @@
         <v>18</v>
       </c>
       <c r="D162" t="str">
-        <f>_xlfn.CONCAT(B162,C162)</f>
+        <f t="shared" si="2"/>
         <v>L6Mexico</v>
       </c>
       <c r="E162">
@@ -3469,7 +3466,7 @@
         <v>19</v>
       </c>
       <c r="D163" t="str">
-        <f>_xlfn.CONCAT(B163,C163)</f>
+        <f t="shared" si="2"/>
         <v>L6Netherlands</v>
       </c>
       <c r="E163">
@@ -3487,7 +3484,7 @@
         <v>38</v>
       </c>
       <c r="D164" t="str">
-        <f>_xlfn.CONCAT(B164,C164)</f>
+        <f t="shared" si="2"/>
         <v>L6P.R.C.</v>
       </c>
       <c r="E164">
@@ -3505,7 +3502,7 @@
         <v>20</v>
       </c>
       <c r="D165" t="str">
-        <f>_xlfn.CONCAT(B165,C165)</f>
+        <f t="shared" si="2"/>
         <v>L6Philippines</v>
       </c>
       <c r="E165">
@@ -3523,7 +3520,7 @@
         <v>40</v>
       </c>
       <c r="D166" t="str">
-        <f>_xlfn.CONCAT(B166,C166)</f>
+        <f t="shared" si="2"/>
         <v>L6Philippines 1</v>
       </c>
       <c r="E166">
@@ -3541,7 +3538,7 @@
         <v>21</v>
       </c>
       <c r="D167" t="str">
-        <f>_xlfn.CONCAT(B167,C167)</f>
+        <f t="shared" si="2"/>
         <v>L6Poland</v>
       </c>
       <c r="E167">
@@ -3559,7 +3556,7 @@
         <v>22</v>
       </c>
       <c r="D168" t="str">
-        <f>_xlfn.CONCAT(B168,C168)</f>
+        <f t="shared" si="2"/>
         <v>L6Puerto Rico</v>
       </c>
       <c r="E168">
@@ -3577,7 +3574,7 @@
         <v>23</v>
       </c>
       <c r="D169" t="str">
-        <f>_xlfn.CONCAT(B169,C169)</f>
+        <f t="shared" si="2"/>
         <v>L6Romania</v>
       </c>
       <c r="E169">
@@ -3595,7 +3592,7 @@
         <v>24</v>
       </c>
       <c r="D170" t="str">
-        <f>_xlfn.CONCAT(B170,C170)</f>
+        <f t="shared" si="2"/>
         <v>L6Saudi Arabia</v>
       </c>
       <c r="E170">
@@ -3613,7 +3610,7 @@
         <v>25</v>
       </c>
       <c r="D171" t="str">
-        <f>_xlfn.CONCAT(B171,C171)</f>
+        <f t="shared" si="2"/>
         <v>L6Serbia</v>
       </c>
       <c r="E171">
@@ -3631,7 +3628,7 @@
         <v>26</v>
       </c>
       <c r="D172" t="str">
-        <f>_xlfn.CONCAT(B172,C172)</f>
+        <f t="shared" si="2"/>
         <v>L6Singapore</v>
       </c>
       <c r="E172">
@@ -3649,7 +3646,7 @@
         <v>27</v>
       </c>
       <c r="D173" t="str">
-        <f>_xlfn.CONCAT(B173,C173)</f>
+        <f t="shared" si="2"/>
         <v>L6Slovakia</v>
       </c>
       <c r="E173">
@@ -3667,7 +3664,7 @@
         <v>28</v>
       </c>
       <c r="D174" t="str">
-        <f>_xlfn.CONCAT(B174,C174)</f>
+        <f t="shared" si="2"/>
         <v>L6Spain</v>
       </c>
       <c r="E174">
@@ -3685,7 +3682,7 @@
         <v>39</v>
       </c>
       <c r="D175" t="str">
-        <f>_xlfn.CONCAT(B175,C175)</f>
+        <f t="shared" si="2"/>
         <v>L6United Arab Emirates</v>
       </c>
       <c r="E175">
@@ -3703,7 +3700,7 @@
         <v>29</v>
       </c>
       <c r="D176" t="str">
-        <f>_xlfn.CONCAT(B176,C176)</f>
+        <f t="shared" si="2"/>
         <v>L6United Kingdom</v>
       </c>
       <c r="E176">
@@ -3721,7 +3718,7 @@
         <v>30</v>
       </c>
       <c r="D177" t="str">
-        <f>_xlfn.CONCAT(B177,C177)</f>
+        <f t="shared" si="2"/>
         <v>L6United States</v>
       </c>
       <c r="E177">
@@ -3739,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="D178" t="str">
-        <f>_xlfn.CONCAT(B178,C178)</f>
+        <f t="shared" si="2"/>
         <v>L7Argentina</v>
       </c>
       <c r="E178">
@@ -3757,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="D179" t="str">
-        <f>_xlfn.CONCAT(B179,C179)</f>
+        <f t="shared" si="2"/>
         <v>L7Australia</v>
       </c>
       <c r="E179">
@@ -3775,7 +3772,7 @@
         <v>2</v>
       </c>
       <c r="D180" t="str">
-        <f>_xlfn.CONCAT(B180,C180)</f>
+        <f t="shared" si="2"/>
         <v>L7Austria</v>
       </c>
       <c r="E180">
@@ -3793,7 +3790,7 @@
         <v>3</v>
       </c>
       <c r="D181" t="str">
-        <f>_xlfn.CONCAT(B181,C181)</f>
+        <f t="shared" si="2"/>
         <v>L7Belgium</v>
       </c>
       <c r="E181">
@@ -3811,7 +3808,7 @@
         <v>37</v>
       </c>
       <c r="D182" t="str">
-        <f>_xlfn.CONCAT(B182,C182)</f>
+        <f t="shared" si="2"/>
         <v>L7Brazil</v>
       </c>
       <c r="E182">
@@ -3829,7 +3826,7 @@
         <v>4</v>
       </c>
       <c r="D183" t="str">
-        <f>_xlfn.CONCAT(B183,C183)</f>
+        <f t="shared" si="2"/>
         <v>L7Brazil 2</v>
       </c>
       <c r="E183">
@@ -3847,7 +3844,7 @@
         <v>5</v>
       </c>
       <c r="D184" t="str">
-        <f>_xlfn.CONCAT(B184,C184)</f>
+        <f t="shared" si="2"/>
         <v>L7Bulgaria</v>
       </c>
       <c r="E184">
@@ -3865,7 +3862,7 @@
         <v>6</v>
       </c>
       <c r="D185" t="str">
-        <f>_xlfn.CONCAT(B185,C185)</f>
+        <f t="shared" si="2"/>
         <v>L7Canada</v>
       </c>
       <c r="E185">
@@ -3883,7 +3880,7 @@
         <v>7</v>
       </c>
       <c r="D186" t="str">
-        <f>_xlfn.CONCAT(B186,C186)</f>
+        <f t="shared" si="2"/>
         <v>L7China 2</v>
       </c>
       <c r="E186">
@@ -3901,7 +3898,7 @@
         <v>8</v>
       </c>
       <c r="D187" t="str">
-        <f>_xlfn.CONCAT(B187,C187)</f>
+        <f t="shared" si="2"/>
         <v>L7Costa Rica</v>
       </c>
       <c r="E187">
@@ -3919,7 +3916,7 @@
         <v>9</v>
       </c>
       <c r="D188" t="str">
-        <f>_xlfn.CONCAT(B188,C188)</f>
+        <f t="shared" si="2"/>
         <v>L7France</v>
       </c>
       <c r="E188">
@@ -3937,7 +3934,7 @@
         <v>10</v>
       </c>
       <c r="D189" t="str">
-        <f>_xlfn.CONCAT(B189,C189)</f>
+        <f t="shared" si="2"/>
         <v>L7Germany</v>
       </c>
       <c r="E189">
@@ -3955,7 +3952,7 @@
         <v>11</v>
       </c>
       <c r="D190" t="str">
-        <f>_xlfn.CONCAT(B190,C190)</f>
+        <f t="shared" si="2"/>
         <v>L7Greece</v>
       </c>
       <c r="E190">
@@ -3973,7 +3970,7 @@
         <v>12</v>
       </c>
       <c r="D191" t="str">
-        <f>_xlfn.CONCAT(B191,C191)</f>
+        <f t="shared" si="2"/>
         <v>L7India</v>
       </c>
       <c r="E191">
@@ -3991,7 +3988,7 @@
         <v>13</v>
       </c>
       <c r="D192" t="str">
-        <f>_xlfn.CONCAT(B192,C192)</f>
+        <f t="shared" si="2"/>
         <v>L7Ireland</v>
       </c>
       <c r="E192">
@@ -4009,7 +4006,7 @@
         <v>14</v>
       </c>
       <c r="D193" t="str">
-        <f>_xlfn.CONCAT(B193,C193)</f>
+        <f t="shared" si="2"/>
         <v>L7Israel</v>
       </c>
       <c r="E193">
@@ -4027,7 +4024,7 @@
         <v>15</v>
       </c>
       <c r="D194" t="str">
-        <f>_xlfn.CONCAT(B194,C194)</f>
+        <f t="shared" ref="D194:D212" si="3">_xlfn.CONCAT(B194,C194)</f>
         <v>L7Italy</v>
       </c>
       <c r="E194">
@@ -4045,7 +4042,7 @@
         <v>16</v>
       </c>
       <c r="D195" t="str">
-        <f>_xlfn.CONCAT(B195,C195)</f>
+        <f t="shared" si="3"/>
         <v>L7Japan</v>
       </c>
       <c r="E195">
@@ -4063,7 +4060,7 @@
         <v>17</v>
       </c>
       <c r="D196" t="str">
-        <f>_xlfn.CONCAT(B196,C196)</f>
+        <f t="shared" si="3"/>
         <v>L7Malaysia</v>
       </c>
       <c r="E196">
@@ -4081,7 +4078,7 @@
         <v>18</v>
       </c>
       <c r="D197" t="str">
-        <f>_xlfn.CONCAT(B197,C197)</f>
+        <f t="shared" si="3"/>
         <v>L7Mexico</v>
       </c>
       <c r="E197">
@@ -4099,7 +4096,7 @@
         <v>19</v>
       </c>
       <c r="D198" t="str">
-        <f>_xlfn.CONCAT(B198,C198)</f>
+        <f t="shared" si="3"/>
         <v>L7Netherlands</v>
       </c>
       <c r="E198">
@@ -4117,7 +4114,7 @@
         <v>38</v>
       </c>
       <c r="D199" t="str">
-        <f>_xlfn.CONCAT(B199,C199)</f>
+        <f t="shared" si="3"/>
         <v>L7P.R.C.</v>
       </c>
       <c r="E199">
@@ -4135,7 +4132,7 @@
         <v>20</v>
       </c>
       <c r="D200" t="str">
-        <f>_xlfn.CONCAT(B200,C200)</f>
+        <f t="shared" si="3"/>
         <v>L7Philippines</v>
       </c>
       <c r="E200">
@@ -4153,7 +4150,7 @@
         <v>40</v>
       </c>
       <c r="D201" t="str">
-        <f>_xlfn.CONCAT(B201,C201)</f>
+        <f t="shared" si="3"/>
         <v>L7Philippines 1</v>
       </c>
       <c r="E201">
@@ -4171,7 +4168,7 @@
         <v>21</v>
       </c>
       <c r="D202" t="str">
-        <f>_xlfn.CONCAT(B202,C202)</f>
+        <f t="shared" si="3"/>
         <v>L7Poland</v>
       </c>
       <c r="E202">
@@ -4189,7 +4186,7 @@
         <v>22</v>
       </c>
       <c r="D203" t="str">
-        <f>_xlfn.CONCAT(B203,C203)</f>
+        <f t="shared" si="3"/>
         <v>L7Puerto Rico</v>
       </c>
       <c r="E203">
@@ -4207,7 +4204,7 @@
         <v>23</v>
       </c>
       <c r="D204" t="str">
-        <f>_xlfn.CONCAT(B204,C204)</f>
+        <f t="shared" si="3"/>
         <v>L7Romania</v>
       </c>
       <c r="E204">
@@ -4225,7 +4222,7 @@
         <v>24</v>
       </c>
       <c r="D205" t="str">
-        <f>_xlfn.CONCAT(B205,C205)</f>
+        <f t="shared" si="3"/>
         <v>L7Saudi Arabia</v>
       </c>
       <c r="E205">
@@ -4243,7 +4240,7 @@
         <v>25</v>
       </c>
       <c r="D206" t="str">
-        <f>_xlfn.CONCAT(B206,C206)</f>
+        <f t="shared" si="3"/>
         <v>L7Serbia</v>
       </c>
       <c r="E206">
@@ -4261,7 +4258,7 @@
         <v>26</v>
       </c>
       <c r="D207" t="str">
-        <f>_xlfn.CONCAT(B207,C207)</f>
+        <f t="shared" si="3"/>
         <v>L7Singapore</v>
       </c>
       <c r="E207">
@@ -4279,7 +4276,7 @@
         <v>27</v>
       </c>
       <c r="D208" t="str">
-        <f>_xlfn.CONCAT(B208,C208)</f>
+        <f t="shared" si="3"/>
         <v>L7Slovakia</v>
       </c>
       <c r="E208">
@@ -4297,7 +4294,7 @@
         <v>28</v>
       </c>
       <c r="D209" t="str">
-        <f>_xlfn.CONCAT(B209,C209)</f>
+        <f t="shared" si="3"/>
         <v>L7Spain</v>
       </c>
       <c r="E209">
@@ -4315,7 +4312,7 @@
         <v>39</v>
       </c>
       <c r="D210" t="str">
-        <f>_xlfn.CONCAT(B210,C210)</f>
+        <f t="shared" si="3"/>
         <v>L7United Arab Emirates</v>
       </c>
       <c r="E210">
@@ -4333,7 +4330,7 @@
         <v>29</v>
       </c>
       <c r="D211" t="str">
-        <f>_xlfn.CONCAT(B211,C211)</f>
+        <f t="shared" si="3"/>
         <v>L7United Kingdom</v>
       </c>
       <c r="E211">
@@ -4351,7 +4348,7 @@
         <v>30</v>
       </c>
       <c r="D212" t="str">
-        <f>_xlfn.CONCAT(B212,C212)</f>
+        <f t="shared" si="3"/>
         <v>L7United States</v>
       </c>
       <c r="E212">

</xml_diff>